<commit_message>
Added sample machine learning scripts
</commit_message>
<xml_diff>
--- a/sampleData.xlsx
+++ b/sampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TestCode\csat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69CC211-D7C1-464C-A1A0-5088F12A6E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488BBCDC-2F4C-40A0-B7EF-56F8A58F1F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="1980" windowWidth="23580" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
-    <t>Responses</t>
-  </si>
-  <si>
     <t>The product exceeded my expectations. It's a game-changer for me.</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t xml:space="preserve">    The product arrived earlier than expected, which was great.</t>
+  </si>
+  <si>
+    <t>Response</t>
   </si>
 </sst>
 </file>
@@ -476,9 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -487,207 +485,207 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>